<commit_message>
Modified code according to this week's bestseller list
</commit_message>
<xml_diff>
--- a/total_bestseller_data.xlsx
+++ b/total_bestseller_data.xlsx
@@ -551,7 +551,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>28</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>304314</t>
+          <t>471210</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -590,357 +590,361 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>110050</v>
+        <v>145980</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>9791169794930</t>
+          <t>9791197389450</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>슬램덩크 리소스-THE FIRST SLAM DUNK re:SOURCE</t>
+          <t>1퍼센트 부자의 법칙</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>사이토 히토리</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>나비스쿨(NAVI SCHOOL)</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44973</v>
+        <v>44956</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE FIRST SLAM DUNK re:SOURCE </t>
+          <t xml:space="preserve">齋藤一人の絶對成功する千回の法則 </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>9.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>20,000원</t>
+          <t>17,000원</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>314799</t>
+          <t>191115</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>처세술/삶의 자세</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>20,000</t>
+          <t>17,000</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1,000점</t>
+          <t>850점</t>
         </is>
       </c>
       <c r="P3" t="n">
-        <v>390885</v>
+        <v>116360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>9791191521221</t>
+          <t>9791169794930</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>K 배터리 레볼루션</t>
+          <t>슬램덩크 리소스-THE FIRST SLAM DUNK re:SOURCE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>박순혁</t>
+          <t>이노우에 타케히코</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>지와인</t>
+          <t>대원</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44977</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
+        <v>44973</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">THE FIRST SLAM DUNK re:SOURCE </t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>36</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>19,000원</t>
+          <t>20,000원</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>17,100</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>222228</t>
+          <t>310362</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>경제전망</t>
+          <t>스포츠</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>19,000</t>
+          <t>20,000</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>17,100</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>950점</t>
+          <t>1,000점</t>
         </is>
       </c>
       <c r="P4" t="n">
-        <v>57205</v>
+        <v>360470</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>9791190538510</t>
+          <t>9791191521221</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>만일 내가 인생을 다시 산다면 (10만 부 기념 스페셜 에디션)</t>
+          <t>K 배터리 레볼루션</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>김혜남</t>
+          <t>박순혁</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>메이븐</t>
+          <t>지와인</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44876</v>
+        <v>44977</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>17,200원</t>
+          <t>19,000원</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>15,480</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>693630</t>
+          <t>289359</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>노년 / 죽음</t>
+          <t>경제전망</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>17,200</t>
+          <t>19,000</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>15,480</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>860점</t>
+          <t>950점</t>
         </is>
       </c>
       <c r="P5" t="n">
-        <v>211535</v>
+        <v>67835</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>9791197871269</t>
+          <t>9791190538510</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>주식 시세의 비밀</t>
+          <t>만일 내가 인생을 다시 산다면 (10만 부 기념 스페셜 에디션)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>정재호</t>
+          <t>김혜남</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>프런트페이지</t>
+          <t>메이븐</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44977</v>
+        <v>44876</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>73</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>22,000원</t>
+          <t>17,200원</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>19,800</t>
+          <t>15,480</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>180297</t>
+          <t>688929</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>주식/증권</t>
+          <t>노년 / 죽음</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>22,000</t>
+          <t>17,200</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>19,800</t>
+          <t>15,480</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>1,100점</t>
+          <t>860점</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>109560</v>
+        <v>202180</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>9791197389450</t>
+          <t>9791168473690</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1퍼센트 부자의 법칙</t>
+          <t>세이노의 가르침</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>사이토 히토리</t>
+          <t>세이노</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>나비스쿨(NAVI SCHOOL)</t>
+          <t>데이원</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44956</v>
+        <v>44987</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>17,000원</t>
+          <t>7,200원</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>6,480</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>121959</t>
+          <t>316608</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -950,46 +954,46 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>7,200</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>6,480</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>850점</t>
+          <t>360점</t>
         </is>
       </c>
       <c r="P7" t="n">
-        <v>88070</v>
+        <v>529205</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>9791130697499</t>
+          <t>9791130642147</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>악인론</t>
+          <t>효기심의 권력으로 읽는 세계사 - 유럽편</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>손수현</t>
+          <t>효기심(최영효)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>다산북스</t>
+          <t>다산초당</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44977</v>
+        <v>44988</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
@@ -999,155 +1003,159 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>18,500원</t>
+          <t>19,800원</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>16,650</t>
+          <t>17,820</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>70230</t>
+          <t>65250</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>성공학/경력관리</t>
+          <t>세계사/세계문화</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>18,500</t>
+          <t>19,800</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>16,650</t>
+          <t>17,820</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>920점</t>
+          <t>990점</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>15230</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>9791161571188</t>
+          <t>9791197871269</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>불편한 편의점</t>
+          <t>주식 시세의 비밀</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>김호연</t>
+          <t>정재호</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>나무옆의자</t>
+          <t>프런트페이지</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44306</v>
+        <v>44977</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>14,000원</t>
+          <t>22,000원</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>19,800</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>1175697</t>
+          <t>191778</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>한국 장편소설</t>
+          <t>주식/증권</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>22,000</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>19,800</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>700점</t>
+          <t>1,100점</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>613933</v>
+        <v>107270</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>9791161571379</t>
+          <t>9788997575169</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>불편한 편의점 2</t>
+          <t>원씽 THE ONE THING</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>김호연</t>
+          <t>게리 켈러</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>나무옆의자</t>
+          <t>비즈니스북스</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44783</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
+        <v>41516</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>The One Thing</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>161</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1162,12 +1170,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>751575</t>
+          <t>492360</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>한국 장편소설</t>
+          <t>처세술/삶의 자세</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1186,106 +1194,106 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>222842</v>
+        <v>160813</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>9791156754039</t>
+          <t>9791161571188</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>정세현의 통찰</t>
+          <t>불편한 편의점</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>정세현</t>
+          <t>김호연</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>푸른숲</t>
+          <t>나무옆의자</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44973</v>
+        <v>44306</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>425</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>19,000원</t>
+          <t>14,000원</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>17,100</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>160152</t>
+          <t>1162683</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>정치/외교학 일반</t>
+          <t>한국 장편소설</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>19,000</t>
+          <t>14,000</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>17,100</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>950점</t>
+          <t>700점</t>
         </is>
       </c>
       <c r="P11" t="n">
-        <v>67800</v>
+        <v>601933</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>9791168473690</t>
+          <t>9791161571379</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>세이노의 가르침</t>
+          <t>불편한 편의점 2</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>세이노</t>
+          <t>김호연</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>데이원</t>
+          <t>나무옆의자</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>44987</v>
+        <v>44783</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
@@ -1295,124 +1303,120 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>121</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>7,200원</t>
+          <t>14,000원</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>6,480</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>333843</t>
+          <t>752925</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>처세술/삶의 자세</t>
+          <t>한국 장편소설</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>7,200</t>
+          <t>14,000</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>6,480</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>360점</t>
+          <t>700점</t>
         </is>
       </c>
       <c r="P12" t="n">
-        <v>531995</v>
+        <v>216218</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>9788997575169</t>
+          <t>9791130697499</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>원씽 THE ONE THING</t>
+          <t>악인론</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>게리 켈러</t>
+          <t>손수현</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>비즈니스북스</t>
+          <t>다산북스</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>41516</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>The One Thing</t>
-        </is>
-      </c>
+        <v>44977</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>25</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>14,000원</t>
+          <t>18,500원</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>16,650</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>483786</t>
+          <t>78984</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>처세술/삶의 자세</t>
+          <t>성공학/경력관리</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>18,500</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>16,650</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>700점</t>
+          <t>920점</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>161459</v>
+        <v>15700</v>
       </c>
     </row>
     <row r="14">
@@ -1447,7 +1451,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1462,7 +1466,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>79053</t>
+          <t>94719</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1486,7 +1490,7 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>40850</v>
+        <v>42970</v>
       </c>
     </row>
     <row r="15">
@@ -1521,7 +1525,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>343</t>
+          <t>346</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1536,7 +1540,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>836943</t>
+          <t>841743</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1560,106 +1564,106 @@
         </is>
       </c>
       <c r="P15" t="n">
-        <v>208292</v>
+        <v>205823</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>9788901268880</t>
+          <t>9791168340855</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5천만 원으로 시작하는 미라클 기적의 재개발 재건축</t>
+          <t>내면소통</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>장미진</t>
+          <t>김주환</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>리더스북</t>
+          <t>인플루엔셜</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>44981</v>
+        <v>44984</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>20,000원</t>
+          <t>33,000원</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>29,700</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>47664</t>
+          <t>45720</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>부동산/경매</t>
+          <t>교양으로 읽는 인문</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>20,000</t>
+          <t>33,000</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>29,700</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>1,000점</t>
+          <t>1,650점</t>
         </is>
       </c>
       <c r="P16" t="n">
-        <v>21220</v>
+        <v>32970</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>9791140702589</t>
+          <t>9788936438838</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>당신도 느리게 나이 들 수 있습니다</t>
+          <t>아버지의 해방일지</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>정희원</t>
+          <t>정지아</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>더퀘스트</t>
+          <t>창비</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>44943</v>
+        <v>44806</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
@@ -1669,416 +1673,416 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>207</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>17,800원</t>
+          <t>15,000원</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>13,500</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>145761</t>
+          <t>564471</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>교양으로 읽는 인문</t>
+          <t>한국 장편소설</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>17,800</t>
+          <t>15,000</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>13,500</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>890점</t>
+          <t>750점</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>75715</v>
+        <v>329013</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>9788936438838</t>
+          <t>9791156754039</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>아버지의 해방일지</t>
+          <t>정세현의 통찰</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>정지아</t>
+          <t>정세현</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>창비</t>
+          <t>푸른숲</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>44806</v>
+        <v>44973</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>202</t>
+          <t>14</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>15,000원</t>
+          <t>19,000원</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>567324</t>
+          <t>164592</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>한국 장편소설</t>
+          <t>정치/외교학 일반</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>15,000</t>
+          <t>19,000</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>750점</t>
+          <t>950점</t>
         </is>
       </c>
       <c r="P18" t="n">
-        <v>333707</v>
+        <v>59690</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>9788950934552</t>
+          <t>9791140702589</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Go Go 카카오프렌즈 27 스위스</t>
+          <t>당신도 느리게 나이 들 수 있습니다</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>김미영</t>
+          <t>정희원</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>아울북</t>
+          <t>더퀘스트</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44972</v>
+        <v>44943</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>61</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>14,800원</t>
+          <t>17,800원</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>13,320</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>65607</t>
+          <t>148299</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>1-2학년 학습만화</t>
+          <t>교양으로 읽는 인문</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>14,800</t>
+          <t>17,800</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>13,320</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>740점</t>
+          <t>890점</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>30540</v>
+        <v>77190</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>9788950941574</t>
+          <t>9788917238549</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>그리스 로마 신화 32</t>
+          <t xml:space="preserve">ETS 토익 정기시험 기출문제집 1000 Vol.3 READING 리딩 </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>박시연</t>
+          <t>ETS</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>아울북</t>
+          <t>YBM(와이비엠)</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>44972</v>
+        <v>44543</v>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>15,000원</t>
+          <t>17,800원</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>56742</t>
+          <t>490212</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1-2학년 신화/전설</t>
+          <t>독해/문법/RC</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>15,000</t>
+          <t>17,800</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>750점</t>
+          <t>890점</t>
         </is>
       </c>
       <c r="P20" t="n">
-        <v>30160</v>
+        <v>197542</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>9791190382915</t>
+          <t>9791169305044</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>생에 감사해</t>
+          <t xml:space="preserve">내가 죽기로 결심한 것은 4 </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>김혜자</t>
+          <t>YUJU</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>수오서재</t>
+          <t xml:space="preserve">네이버웹툰유한회사 </t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>44917</v>
+        <v>44990</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>17,000원</t>
+          <t>16,000원</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>277443</t>
+          <t>34590</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t xml:space="preserve">명사/연예인 에세이 </t>
+          <t xml:space="preserve">네이버 연재 </t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>16,000</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>850점</t>
+          <t>800점</t>
         </is>
       </c>
       <c r="P21" t="n">
-        <v>125545</v>
+        <v>64760</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>9788917238549</t>
+          <t>9791190382915</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">ETS 토익 정기시험 기출문제집 1000 Vol.3 READING 리딩 </t>
+          <t>생에 감사해</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ETS</t>
+          <t>김혜자</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>YBM(와이비엠)</t>
+          <t>수오서재</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>44543</v>
+        <v>44917</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>25</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>17,800원</t>
+          <t>17,000원</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>492918</t>
+          <t>265008</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>독해/문법/RC</t>
+          <t xml:space="preserve">명사/연예인 에세이 </t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>17,800</t>
+          <t>17,000</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>890점</t>
+          <t>850점</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>199311</v>
+        <v>121445</v>
       </c>
     </row>
     <row r="23">
@@ -2113,7 +2117,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>77</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2128,7 +2132,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>458283</t>
+          <t>456111</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2152,732 +2156,712 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>185206</v>
+        <v>182645</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>9791191043297</t>
+          <t>9791169305037</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>오늘 밤, 세계에서 이 사랑이 사라진다 해도</t>
+          <t xml:space="preserve">내가 죽기로 결심한 것은 3 </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>이치조 미사키</t>
+          <t>YUJU</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>모모</t>
+          <t xml:space="preserve">네이버웹툰유한회사 </t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>44375</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>今夜,世界からこの戀が消えても</t>
-        </is>
-      </c>
+        <v>44990</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>77</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>14,000원</t>
+          <t>16,000원</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>425508</t>
+          <t>34080</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>연애/사랑소설</t>
+          <t xml:space="preserve">네이버 연재 </t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>16,000</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>700점</t>
+          <t>800점</t>
         </is>
       </c>
       <c r="P24" t="n">
-        <v>154399</v>
+        <v>64680</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>9791192625300</t>
+          <t>9791191043297</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">이은경쌤의 초등어휘일력 365 </t>
+          <t>오늘 밤, 세계에서 이 사랑이 사라진다 해도</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>이은경</t>
+          <t>이치조 미사키</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>포레스트북스</t>
+          <t>모모</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>44862</v>
-      </c>
-      <c r="F25" t="inlineStr"/>
+        <v>44375</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>今夜,世界からこの戀が消えても</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>9.9</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>134</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>18,800원</t>
+          <t>14,000원</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>16,920</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>341076</t>
+          <t>419454</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>독서교육</t>
+          <t>연애/사랑소설</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>18,800</t>
+          <t>14,000</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>16,920</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>940점</t>
+          <t>700점</t>
         </is>
       </c>
       <c r="P25" t="n">
-        <v>83228</v>
+        <v>150096</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>9791133487516</t>
+          <t>9791198179913</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 1</t>
+          <t>설민석의 한국사 대모험 24</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>설민석</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>단꿈아이</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>43336</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  1 </t>
-        </is>
-      </c>
+        <v>44984</v>
+      </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>134</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>13,000원</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>294603</t>
+          <t>33300</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>1-2학년 학습만화</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>13,000</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>650점</t>
         </is>
       </c>
       <c r="P26" t="n">
-        <v>158331</v>
+        <v>18420</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>9791197647666</t>
+          <t>9788950934552</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>기분이 태도가 되지 말자</t>
+          <t>Go Go 카카오프렌즈 27 스위스</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>김수현</t>
+          <t>김미영</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>하이스트</t>
+          <t>아울북</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>44890</v>
+        <v>44972</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>16,000원</t>
+          <t>14,800원</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>14,400</t>
+          <t>13,320</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>173865</t>
+          <t>76086</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>삶의 자세와 지혜</t>
+          <t>1-2학년 학습만화</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>16,000</t>
+          <t>14,800</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>14,400</t>
+          <t>13,320</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>800점</t>
+          <t>740점</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>39490</v>
+        <v>29290</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>9791158883591</t>
+          <t>9791158773120</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>부자 아빠 가난한 아빠 20주년 특별 기념판</t>
+          <t>건강과 다이어트를 동시에 잡는 7대 3의 법칙 채소·과일식</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>로버트 기요사키</t>
+          <t>조승우</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>민음인</t>
+          <t>바이북스</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>43153</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Rich Dad Poor Dad</t>
-        </is>
-      </c>
+        <v>44854</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>50</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>17,000원</t>
+          <t>19,000원</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>424254</t>
+          <t>97581</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>재테크일반</t>
+          <t>건강에세이/건강기타</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>19,000</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>850점</t>
+          <t>950점</t>
         </is>
       </c>
       <c r="P28" t="n">
-        <v>130974</v>
+        <v>30543</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>9791189327156</t>
+          <t>9791169794183</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>물고기는 존재하지 않는다</t>
+          <t>타키 포오의 이세계 여행사 1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>룰루 밀러</t>
+          <t>캐릭온TV</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>곰출판</t>
+          <t>대원씨아이(단행)(대원키즈)</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>44547</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Why Fish Don't Exist: A Story of Loss, Love, and the Hidden Order of Life</t>
-        </is>
-      </c>
+        <v>44978</v>
+      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>50</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>17,000원</t>
+          <t>13,000원</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>488874</t>
+          <t>38544</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>생물학</t>
+          <t>1-2학년 애니메이션/영화드라마 원작</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>13,000</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>850점</t>
+          <t>650점</t>
         </is>
       </c>
       <c r="P29" t="n">
-        <v>261777</v>
+        <v>11820</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>9791133487707</t>
+          <t>9791192625300</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 20</t>
+          <t xml:space="preserve">이은경쌤의 초등어휘일력 365 </t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>이은경</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>포레스트북스</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>43418</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  20 </t>
-        </is>
-      </c>
+        <v>44862</v>
+      </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
-          <t>9.8</t>
+          <t>9.9</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>49</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>18,800원</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>16,920</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>286851</t>
+          <t>343023</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>독서교육</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>18,800</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>16,920</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>940점</t>
         </is>
       </c>
       <c r="P30" t="n">
-        <v>146456</v>
+        <v>82830</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>9791133487547</t>
+          <t>9791158883591</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 4</t>
+          <t>부자 아빠 가난한 아빠 20주년 특별 기념판</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>로버트 기요사키</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>민음인</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>43336</v>
+        <v>43153</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>SLAM DUNK 新裝再編版  4</t>
+          <t>Rich Dad Poor Dad</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>212</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>17,000원</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>282714</t>
+          <t>420315</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>재테크일반</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>17,000</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>850점</t>
         </is>
       </c>
       <c r="P31" t="n">
-        <v>144618</v>
+        <v>129498</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>9791133487530</t>
+          <t>9791189327156</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 3</t>
+          <t>물고기는 존재하지 않는다</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>룰루 밀러</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>곰출판</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>43336</v>
+        <v>44547</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>SLAM DUNK 新裝再編版  3</t>
+          <t>Why Fish Don't Exist: A Story of Loss, Love, and the Hidden Order of Life</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>243</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>17,000원</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>280515</t>
+          <t>478287</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>생물학</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>17,000</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>850점</t>
         </is>
       </c>
       <c r="P32" t="n">
-        <v>150795</v>
+        <v>260506</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>9791133487691</t>
+          <t>9791168181304</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 19</t>
+          <t>2023 이유진 국어 필사즉생 모의고사 백일기도 3 - 실전유형</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>이유진</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>고시동네</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>43418</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  19 </t>
-        </is>
-      </c>
+        <v>44977</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
           <t>10.0</t>
@@ -2885,149 +2869,145 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>16,000원</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>278823</t>
+          <t>52788</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t xml:space="preserve">문제집/모의고사 </t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>16,000</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>800점</t>
         </is>
       </c>
       <c r="P33" t="n">
-        <v>144917</v>
+        <v>25530</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>9791133487677</t>
+          <t>9788901268880</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 17</t>
+          <t>5천만 원으로 시작하는 미라클 기적의 재개발 재건축</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>장미진</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>리더스북</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>43418</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  17 </t>
-        </is>
-      </c>
+        <v>44981</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
-          <t>9.8</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>20,000원</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>276318</t>
+          <t>55830</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>부동산/경매</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>20,000</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>1,000점</t>
         </is>
       </c>
       <c r="P34" t="n">
-        <v>141162</v>
+        <v>20390</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>9791157062805</t>
+          <t>9788950941574</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>미스터 프레지던트</t>
+          <t>그리스 로마 신화 32</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>탁현민</t>
+          <t>박시연</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>메디치미디어</t>
+          <t>아울북</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>44944</v>
+        <v>44972</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
@@ -3037,291 +3017,279 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>22,000원</t>
+          <t>15,000원</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>19,800</t>
+          <t>13,500</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>244200</t>
+          <t>66432</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>신문/방송</t>
+          <t>1-2학년 신화/전설</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>22,000</t>
+          <t>15,000</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>19,800</t>
+          <t>13,500</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>1,100점</t>
+          <t>750점</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>92105</v>
+        <v>27450</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>9791133487561</t>
+          <t>9788988474846</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 6</t>
+          <t>SQL 자격검정 실전문제</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>한국데이터진흥원</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>한국데이터산업진흥원</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>43336</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>SLAM DUNK 新裝再編版  6</t>
-        </is>
-      </c>
+        <v>43962</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>51</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>18,000원</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>279723</t>
+          <t>105831</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>SQL Server</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>0점</t>
         </is>
       </c>
       <c r="P36" t="n">
-        <v>142977</v>
+        <v>58157</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>9791133487660</t>
+          <t>9788936448370</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 16</t>
+          <t>고양이 해결사 깜냥 5</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>홍민정</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>창비</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>43418</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  16 </t>
-        </is>
-      </c>
+        <v>44981</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>49,500</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>51</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>11,000원</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>9,900</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>275895</t>
+          <t>27300</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>1-2학년 창작동화</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>11,000</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>9,900</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>550점</t>
         </is>
       </c>
       <c r="P37" t="n">
-        <v>140955</v>
+        <v>45070</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>9791133487653</t>
+          <t>9788956608556</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 15</t>
+          <t>구의 증명</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>최진영</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>은행나무</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>43418</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  15 </t>
-        </is>
-      </c>
+        <v>42093</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>67</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>7,500원</t>
+          <t>8,000원</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>6,750</t>
+          <t>7,200</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>275031</t>
+          <t>156027</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>한국 장편소설</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>7,500</t>
+          <t>8,000</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>6,750</t>
+          <t>7,200</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>370점</t>
+          <t>400점</t>
         </is>
       </c>
       <c r="P38" t="n">
-        <v>137275</v>
+        <v>88017</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>9791133487578</t>
+          <t>9791133487523</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 7</t>
+          <t>슬램덩크 신장재편판 2</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3335,36 +3303,36 @@
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>43361</v>
+        <v>43336</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>SLAM DUNK 新裝再編版  7</t>
+          <t xml:space="preserve">SLAM DUNK 新裝再編版 2 </t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>71</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>7,500원</t>
+          <t>6,500원</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>6,750</t>
+          <t>5,850</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>271734</t>
+          <t>291171</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3374,32 +3342,32 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>7,500</t>
+          <t>6,500</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>6,750</t>
+          <t>5,850</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>370점</t>
+          <t>320점</t>
         </is>
       </c>
       <c r="P39" t="n">
-        <v>139903</v>
+        <v>153314</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>9791133487554</t>
+          <t>9791133487516</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 5</t>
+          <t>슬램덩크 신장재편판 1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3417,17 +3385,17 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>SLAM DUNK 新裝再編版  5</t>
+          <t xml:space="preserve">SLAM DUNK 新裝再編版  1 </t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>9.8</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>91</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -3442,7 +3410,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>283539</t>
+          <t>296085</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3466,18 +3434,18 @@
         </is>
       </c>
       <c r="P40" t="n">
-        <v>145323</v>
+        <v>156584</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>9791133487684</t>
+          <t>9791133487547</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 18</t>
+          <t>슬램덩크 신장재편판 4</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -3491,36 +3459,36 @@
         </is>
       </c>
       <c r="E41" s="2" t="n">
-        <v>43418</v>
+        <v>43336</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  18 </t>
+          <t>SLAM DUNK 新裝再編版  4</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>9.8</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>63</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>6,500원</t>
+          <t>7,000원</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>5,850</t>
+          <t>6,300</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>277053</t>
+          <t>285882</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3530,21 +3498,21 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>6,500</t>
+          <t>7,000</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>5,850</t>
+          <t>6,300</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>320점</t>
+          <t>350점</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>140966</v>
+        <v>141019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started to clean and analyze the data. Started by grouping YES24 genres together than getting the mean and median of yes24 related columns for each genre.
</commit_message>
<xml_diff>
--- a/total_bestseller_data.xlsx
+++ b/total_bestseller_data.xlsx
@@ -566,7 +566,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>471210</t>
+          <t>516042</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>145980</v>
+        <v>154420</v>
       </c>
     </row>
     <row r="3">
@@ -644,7 +644,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>191115</t>
+          <t>200355</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>116360</v>
+        <v>120130</v>
       </c>
     </row>
     <row r="4">
@@ -707,7 +707,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>38</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>310362</t>
+          <t>311589</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>360470</v>
+        <v>356655</v>
       </c>
     </row>
     <row r="5">
@@ -796,7 +796,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>289359</t>
+          <t>298755</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -820,155 +820,155 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>67835</v>
+        <v>70815</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>9791190538510</t>
+          <t>9791168473690</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>만일 내가 인생을 다시 산다면 (10만 부 기념 스페셜 에디션)</t>
+          <t>세이노의 가르침</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>김혜남</t>
+          <t>세이노</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>메이븐</t>
+          <t>데이원</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44876</v>
+        <v>44987</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>11</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>17,200원</t>
+          <t>7,200원</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>15,480</t>
+          <t>6,480</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>688929</t>
+          <t>320472</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>노년 / 죽음</t>
+          <t>처세술/삶의 자세</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>17,200</t>
+          <t>7,200</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>15,480</t>
+          <t>6,480</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>860점</t>
+          <t>360점</t>
         </is>
       </c>
       <c r="P6" t="n">
-        <v>202180</v>
+        <v>541195</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>9791168473690</t>
+          <t>9791190538510</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>세이노의 가르침</t>
+          <t>만일 내가 인생을 다시 산다면 (10만 부 기념 스페셜 에디션)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>세이노</t>
+          <t>김혜남</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>데이원</t>
+          <t>메이븐</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44987</v>
+        <v>44876</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>75</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>7,200원</t>
+          <t>17,200원</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>6,480</t>
+          <t>15,480</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>316608</t>
+          <t>685509</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>처세술/삶의 자세</t>
+          <t>노년 / 죽음</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>7,200</t>
+          <t>17,200</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>6,480</t>
+          <t>15,480</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>360점</t>
+          <t>860점</t>
         </is>
       </c>
       <c r="P7" t="n">
-        <v>529205</v>
+        <v>200945</v>
       </c>
     </row>
     <row r="8">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>65250</t>
+          <t>71100</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1026,136 +1026,122 @@
           <t>세계사/세계문화</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>19,800</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>17,820</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>990점</t>
-        </is>
-      </c>
-      <c r="P8" t="n">
-        <v>14000</v>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>9791197871269</t>
+          <t>9788997575169</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>주식 시세의 비밀</t>
+          <t>원씽 THE ONE THING</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>정재호</t>
+          <t>게리 켈러</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>프런트페이지</t>
+          <t>비즈니스북스</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44977</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
+        <v>41516</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>The One Thing</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>162</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>22,000원</t>
+          <t>14,000원</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>19,800</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>191778</t>
+          <t>490854</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>주식/증권</t>
+          <t>처세술/삶의 자세</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>22,000</t>
+          <t>14,000</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>19,800</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>1,100점</t>
+          <t>700점</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>107270</v>
+        <v>159896</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>9788997575169</t>
+          <t>9791161571188</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>원씽 THE ONE THING</t>
+          <t>불편한 편의점</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>게리 켈러</t>
+          <t>김호연</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>비즈니스북스</t>
+          <t>나무옆의자</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>41516</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>The One Thing</t>
-        </is>
-      </c>
+        <v>44306</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>161</t>
+          <t>429</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1170,12 +1156,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>492360</t>
+          <t>1157388</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>처세술/삶의 자세</t>
+          <t>한국 장편소설</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1194,264 +1180,250 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>160813</v>
+        <v>602266</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>9791161571188</t>
+          <t>9791197871269</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>불편한 편의점</t>
+          <t>주식 시세의 비밀</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>김호연</t>
+          <t>정재호</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>나무옆의자</t>
+          <t>프런트페이지</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44306</v>
+        <v>44977</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>425</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>14,000원</t>
+          <t>22,000원</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>19,800</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>1162683</t>
+          <t>195501</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>한국 장편소설</t>
+          <t>주식/증권</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>22,000</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>19,800</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>700점</t>
+          <t>1,100점</t>
         </is>
       </c>
       <c r="P11" t="n">
-        <v>601933</v>
+        <v>104470</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>9791161571379</t>
+          <t>9791168340855</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>불편한 편의점 2</t>
+          <t>내면소통</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>김호연</t>
+          <t>김주환</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>나무옆의자</t>
+          <t>인플루엔셜</t>
         </is>
       </c>
       <c r="E12" s="2" t="n">
-        <v>44783</v>
+        <v>44984</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>14,000원</t>
+          <t>33,000원</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>29,700</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>752925</t>
+          <t>54870</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>한국 장편소설</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>14,000</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>12,600</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>700점</t>
-        </is>
-      </c>
-      <c r="P12" t="n">
-        <v>216218</v>
-      </c>
+          <t>교양으로 읽는 인문</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>9791130697499</t>
+          <t>9791161571379</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>악인론</t>
+          <t>불편한 편의점 2</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>손수현</t>
+          <t>김호연</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>다산북스</t>
+          <t>나무옆의자</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>44977</v>
+        <v>44783</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>121</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>18,500원</t>
+          <t>14,000원</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>16,650</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>78984</t>
+          <t>751095</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>성공학/경력관리</t>
+          <t>한국 장편소설</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>18,500</t>
+          <t>14,000</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>16,650</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>920점</t>
+          <t>700점</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>15700</v>
+        <v>216235</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>9791192932057</t>
+          <t>9791198179913</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>챗GPT</t>
+          <t>설민석의 한국사 대모험 24</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>반병현</t>
+          <t>설민석</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>생능북스</t>
+          <t>단꿈아이</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>44972</v>
+        <v>44984</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1466,81 +1438,67 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>94719</t>
+          <t>52680</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>경영전략/경영혁신</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>13,000</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>11,700</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>650점</t>
-        </is>
-      </c>
-      <c r="P14" t="n">
-        <v>42970</v>
-      </c>
+          <t>1-2학년 학습만화</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>9788901260716</t>
+          <t>9791130697499</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>역행자</t>
+          <t>악인론</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>자청</t>
+          <t>손수현</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>웅진지식하우스</t>
+          <t>다산북스</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>44711</v>
+        <v>44977</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>64</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>17,500원</t>
+          <t>18,500원</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>15,750</t>
+          <t>16,650</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>841743</t>
+          <t>80976</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1550,268 +1508,254 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>17,500</t>
+          <t>18,500</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>15,750</t>
+          <t>16,650</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>870점</t>
+          <t>920점</t>
         </is>
       </c>
       <c r="P15" t="n">
-        <v>205823</v>
+        <v>15940</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>9791168340855</t>
+          <t>9788901260716</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>내면소통</t>
+          <t>역행자</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>김주환</t>
+          <t>자청</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>인플루엔셜</t>
+          <t>웅진지식하우스</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>44984</v>
+        <v>44711</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>349</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>33,000원</t>
+          <t>17,500원</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>29,700</t>
+          <t>15,750</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>45720</t>
+          <t>842058</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>교양으로 읽는 인문</t>
+          <t>성공학/경력관리</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>33,000</t>
+          <t>17,500</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>29,700</t>
+          <t>15,750</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>1,650점</t>
+          <t>870점</t>
         </is>
       </c>
       <c r="P16" t="n">
-        <v>32970</v>
+        <v>204665</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>9788936438838</t>
+          <t>9791192932057</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>아버지의 해방일지</t>
+          <t>챗GPT</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>정지아</t>
+          <t>반병현</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>창비</t>
+          <t>생능북스</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>44806</v>
+        <v>44972</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>207</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>15,000원</t>
+          <t>13,000원</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>564471</t>
+          <t>98457</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>한국 장편소설</t>
+          <t>경영전략/경영혁신</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>15,000</t>
+          <t>13,000</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>750점</t>
+          <t>650점</t>
         </is>
       </c>
       <c r="P17" t="n">
-        <v>329013</v>
+        <v>44100</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>9791156754039</t>
+          <t>9788936448370</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>정세현의 통찰</t>
+          <t>고양이 해결사 깜냥 5</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>정세현</t>
+          <t>홍민정</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>푸른숲</t>
+          <t>창비</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>44973</v>
+        <v>44981</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
-          <t>9.8</t>
+          <t>49,500</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>19,000원</t>
+          <t>11,000원</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>17,100</t>
+          <t>9,900</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>164592</t>
+          <t>39180</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>정치/외교학 일반</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>19,000</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>17,100</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>950점</t>
-        </is>
-      </c>
-      <c r="P18" t="n">
-        <v>59690</v>
-      </c>
+          <t>1-2학년 창작동화</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>9791140702589</t>
+          <t>9788936438838</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>당신도 느리게 나이 들 수 있습니다</t>
+          <t>아버지의 해방일지</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>정희원</t>
+          <t>정지아</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>더퀘스트</t>
+          <t>창비</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44943</v>
+        <v>44806</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
@@ -1821,131 +1765,117 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>207</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>17,800원</t>
+          <t>15,000원</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>13,500</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>148299</t>
+          <t>562650</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>교양으로 읽는 인문</t>
+          <t>한국 장편소설</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>17,800</t>
+          <t>15,000</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>13,500</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>890점</t>
+          <t>750점</t>
         </is>
       </c>
       <c r="P19" t="n">
-        <v>77190</v>
+        <v>327481</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>9788917238549</t>
+          <t>9791169305044</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">ETS 토익 정기시험 기출문제집 1000 Vol.3 READING 리딩 </t>
+          <t xml:space="preserve">내가 죽기로 결심한 것은 4 </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ETS</t>
+          <t>YUJU</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>YBM(와이비엠)</t>
+          <t xml:space="preserve">네이버웹툰유한회사 </t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>44543</v>
+        <v>44990</v>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>207</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>17,800원</t>
+          <t>16,000원</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>14,400</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>490212</t>
+          <t>37230</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>독해/문법/RC</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>17,800</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>16,020</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>890점</t>
-        </is>
-      </c>
-      <c r="P20" t="n">
-        <v>197542</v>
-      </c>
+          <t xml:space="preserve">네이버 연재 </t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>9791169305044</t>
+          <t>9791169305037</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">내가 죽기로 결심한 것은 4 </t>
+          <t xml:space="preserve">내가 죽기로 결심한 것은 3 </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1969,7 +1899,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>207</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1984,7 +1914,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>34590</t>
+          <t>36780</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1992,496 +1922,468 @@
           <t xml:space="preserve">네이버 연재 </t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>16,000</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>14,400</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>800점</t>
-        </is>
-      </c>
-      <c r="P21" t="n">
-        <v>64760</v>
-      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>9791190382915</t>
+          <t>9788917238549</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>생에 감사해</t>
+          <t xml:space="preserve">ETS 토익 정기시험 기출문제집 1000 Vol.3 READING 리딩 </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>김혜자</t>
+          <t>ETS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>수오서재</t>
+          <t>YBM(와이비엠)</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>44917</v>
+        <v>44543</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>17,000원</t>
+          <t>17,800원</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>265008</t>
+          <t>488931</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t xml:space="preserve">명사/연예인 에세이 </t>
+          <t>독해/문법/RC</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>17,800</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>850점</t>
+          <t>890점</t>
         </is>
       </c>
       <c r="P22" t="n">
-        <v>121445</v>
+        <v>200534</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>9788917238532</t>
+          <t>9791169794183</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">ETS 토익 정기시험 기출문제집 1000 Vol.3 LISTENING 리스닝  </t>
+          <t>타키 포오의 이세계 여행사 1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ETS</t>
+          <t>캐릭온TV</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>YBM(와이비엠)</t>
+          <t>대원씨아이(단행)(대원키즈)</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>44543</v>
+        <v>44978</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>17,800원</t>
+          <t>13,000원</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>16,020</t>
+          <t>11,700</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>456111</t>
+          <t>44586</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>청해/LC</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>17,800</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>16,020</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>890점</t>
-        </is>
-      </c>
-      <c r="P23" t="n">
-        <v>182645</v>
-      </c>
+          <t>1-2학년 애니메이션/영화드라마 원작</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>9791169305037</t>
+          <t>9791140702589</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">내가 죽기로 결심한 것은 3 </t>
+          <t>당신도 느리게 나이 들 수 있습니다</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>YUJU</t>
+          <t>정희원</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">네이버웹툰유한회사 </t>
+          <t>더퀘스트</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>44990</v>
+        <v>44943</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
-          <t>14,400</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>62</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>16,000원</t>
+          <t>17,800원</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>14,400</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>34080</t>
+          <t>148533</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t xml:space="preserve">네이버 연재 </t>
+          <t>교양으로 읽는 인문</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>16,000</t>
+          <t>17,800</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>14,400</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>800점</t>
+          <t>890점</t>
         </is>
       </c>
       <c r="P24" t="n">
-        <v>64680</v>
+        <v>79535</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>9791191043297</t>
+          <t>9791190382915</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>오늘 밤, 세계에서 이 사랑이 사라진다 해도</t>
+          <t>생에 감사해</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>이치조 미사키</t>
+          <t>김혜자</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>모모</t>
+          <t>수오서재</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>44375</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>今夜,世界からこの戀が消えても</t>
-        </is>
-      </c>
+        <v>44917</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>26</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>14,000원</t>
+          <t>17,000원</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>419454</t>
+          <t>262707</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>연애/사랑소설</t>
+          <t xml:space="preserve">명사/연예인 에세이 </t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>14,000</t>
+          <t>17,000</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>12,600</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>700점</t>
+          <t>850점</t>
         </is>
       </c>
       <c r="P25" t="n">
-        <v>150096</v>
+        <v>120335</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>9791198179913</t>
+          <t>9788917238532</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>설민석의 한국사 대모험 24</t>
+          <t xml:space="preserve">ETS 토익 정기시험 기출문제집 1000 Vol.3 LISTENING 리스닝  </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>설민석</t>
+          <t>ETS</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>단꿈아이</t>
+          <t>YBM(와이비엠)</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>44984</v>
+        <v>44543</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
-          <t>11,700</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>77</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>13,000원</t>
+          <t>17,800원</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>11,700</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>33300</t>
+          <t>454467</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>1-2학년 학습만화</t>
+          <t>청해/LC</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>13,000</t>
+          <t>17,800</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>11,700</t>
+          <t>16,020</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>650점</t>
+          <t>890점</t>
         </is>
       </c>
       <c r="P26" t="n">
-        <v>18420</v>
+        <v>185759</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>9788950934552</t>
+          <t>9791191043297</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Go Go 카카오프렌즈 27 스위스</t>
+          <t>오늘 밤, 세계에서 이 사랑이 사라진다 해도</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>김미영</t>
+          <t>이치조 미사키</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>아울북</t>
+          <t>모모</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>44972</v>
-      </c>
-      <c r="F27" t="inlineStr"/>
+        <v>44375</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>今夜,世界からこの戀が消えても</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>137</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>14,800원</t>
+          <t>14,000원</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>13,320</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>76086</t>
+          <t>417882</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>1-2학년 학습만화</t>
+          <t>연애/사랑소설</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>14,800</t>
+          <t>14,000</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>13,320</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>740점</t>
+          <t>700점</t>
         </is>
       </c>
       <c r="P27" t="n">
-        <v>29290</v>
+        <v>149310</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>9791158773120</t>
+          <t>9791156754039</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>건강과 다이어트를 동시에 잡는 7대 3의 법칙 채소·과일식</t>
+          <t>정세현의 통찰</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>조승우</t>
+          <t>정세현</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>바이북스</t>
+          <t>푸른숲</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>44854</v>
+        <v>44973</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
@@ -2491,7 +2393,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>20</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2506,12 +2408,12 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>97581</t>
+          <t>165120</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>건강에세이/건강기타</t>
+          <t>정치/외교학 일반</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2530,844 +2432,824 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>30543</v>
+        <v>59260</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>9791169794183</t>
+          <t>9791158883591</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>타키 포오의 이세계 여행사 1</t>
+          <t>부자 아빠 가난한 아빠 20주년 특별 기념판</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>캐릭온TV</t>
+          <t>로버트 기요사키</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>대원씨아이(단행)(대원키즈)</t>
+          <t>민음인</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>44978</v>
-      </c>
-      <c r="F29" t="inlineStr"/>
+        <v>43153</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Rich Dad Poor Dad</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>213</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>13,000원</t>
+          <t>17,000원</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>11,700</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>38544</t>
+          <t>420339</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>1-2학년 애니메이션/영화드라마 원작</t>
+          <t>재테크일반</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>13,000</t>
+          <t>17,000</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>11,700</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>650점</t>
+          <t>850점</t>
         </is>
       </c>
       <c r="P29" t="n">
-        <v>11820</v>
+        <v>129455</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>9791192625300</t>
+          <t>9791133487523</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">이은경쌤의 초등어휘일력 365 </t>
+          <t>슬램덩크 신장재편판 2</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>이은경</t>
+          <t>이노우에 타케히코</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>포레스트북스</t>
+          <t>대원</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>44862</v>
-      </c>
-      <c r="F30" t="inlineStr"/>
+        <v>43336</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SLAM DUNK 新裝再編版 2 </t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>9.9</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>71</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>18,800원</t>
+          <t>6,500원</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>16,920</t>
+          <t>5,850</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>343023</t>
+          <t>293943</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>독서교육</t>
+          <t>스포츠</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>18,800</t>
+          <t>6,500</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>16,920</t>
+          <t>5,850</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>940점</t>
+          <t>320점</t>
         </is>
       </c>
       <c r="P30" t="n">
-        <v>82830</v>
+        <v>152831</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>9791158883591</t>
+          <t>9791192625300</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>부자 아빠 가난한 아빠 20주년 특별 기념판</t>
+          <t xml:space="preserve">이은경쌤의 초등어휘일력 365 </t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>로버트 기요사키</t>
+          <t>이은경</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>민음인</t>
+          <t>포레스트북스</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>43153</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Rich Dad Poor Dad</t>
-        </is>
-      </c>
+        <v>44862</v>
+      </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>9.9</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>49</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>17,000원</t>
+          <t>18,800원</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>16,920</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>420315</t>
+          <t>343233</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>재테크일반</t>
+          <t>독서교육</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>17,000</t>
+          <t>18,800</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>16,920</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>850점</t>
+          <t>940점</t>
         </is>
       </c>
       <c r="P31" t="n">
-        <v>129498</v>
+        <v>82822</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>9791189327156</t>
+          <t>9788950934552</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>물고기는 존재하지 않는다</t>
+          <t>Go Go 카카오프렌즈 27 스위스</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>룰루 밀러</t>
+          <t>김미영</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>곰출판</t>
+          <t>아울북</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>44547</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Why Fish Don't Exist: A Story of Loss, Love, and the Hidden Order of Life</t>
-        </is>
-      </c>
+        <v>44972</v>
+      </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>13</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>17,000원</t>
+          <t>14,800원</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>15,300</t>
+          <t>13,320</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>478287</t>
+          <t>79428</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>생물학</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>17,000</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>15,300</t>
-        </is>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>850점</t>
-        </is>
-      </c>
-      <c r="P32" t="n">
-        <v>260506</v>
-      </c>
+          <t>1-2학년 학습만화</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>9791168181304</t>
+          <t>9791158773120</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2023 이유진 국어 필사즉생 모의고사 백일기도 3 - 실전유형</t>
+          <t>건강과 다이어트를 동시에 잡는 7대 3의 법칙 채소·과일식</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>이유진</t>
+          <t>조승우</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>고시동네</t>
+          <t>바이북스</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>44977</v>
+        <v>44854</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>50</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>16,000원</t>
+          <t>19,000원</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>14,400</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>52788</t>
+          <t>98868</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t xml:space="preserve">문제집/모의고사 </t>
+          <t>건강에세이/건강기타</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>16,000</t>
+          <t>19,000</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>14,400</t>
+          <t>17,100</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>800점</t>
+          <t>950점</t>
         </is>
       </c>
       <c r="P33" t="n">
-        <v>25530</v>
+        <v>31757</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>9788901268880</t>
+          <t>9791133487516</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5천만 원으로 시작하는 미라클 기적의 재개발 재건축</t>
+          <t>슬램덩크 신장재편판 1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>장미진</t>
+          <t>이노우에 타케히코</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>리더스북</t>
+          <t>대원</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>44981</v>
-      </c>
-      <c r="F34" t="inlineStr"/>
+        <v>43336</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SLAM DUNK 新裝再編版  1 </t>
+        </is>
+      </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>91</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>20,000원</t>
+          <t>7,000원</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>6,300</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>55830</t>
+          <t>297693</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>부동산/경매</t>
+          <t>스포츠</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>20,000</t>
+          <t>7,000</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>6,300</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>1,000점</t>
+          <t>350점</t>
         </is>
       </c>
       <c r="P34" t="n">
-        <v>20390</v>
+        <v>156091</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>9788950941574</t>
+          <t>9791133487530</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>그리스 로마 신화 32</t>
+          <t>슬램덩크 신장재편판 3</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>박시연</t>
+          <t>이노우에 타케히코</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>아울북</t>
+          <t>대원</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>44972</v>
-      </c>
-      <c r="F35" t="inlineStr"/>
+        <v>43336</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>SLAM DUNK 新裝再編版  3</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>73</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>15,000원</t>
+          <t>7,000원</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>6,300</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>66432</t>
+          <t>284637</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>1-2학년 신화/전설</t>
+          <t>스포츠</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>15,000</t>
+          <t>7,000</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>13,500</t>
+          <t>6,300</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>750점</t>
+          <t>350점</t>
         </is>
       </c>
       <c r="P35" t="n">
-        <v>27450</v>
+        <v>146722</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>9788988474846</t>
+          <t>9788950970901</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SQL 자격검정 실전문제</t>
+          <t>마법천자문 57</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>한국데이터진흥원</t>
+          <t>유대영</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>한국데이터산업진흥원</t>
+          <t>아울북</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>43962</v>
+        <v>44985</v>
       </c>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>73</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>18,000원</t>
+          <t>14,000원</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>18,000</t>
+          <t>12,600</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>105831</t>
+          <t>30180</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>SQL Server</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>18,000</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>18,000</t>
-        </is>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>0점</t>
-        </is>
-      </c>
-      <c r="P36" t="n">
-        <v>58157</v>
-      </c>
+          <t>1-2학년 학습만화</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>9788936448370</t>
+          <t>9791189327156</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>고양이 해결사 깜냥 5</t>
+          <t>물고기는 존재하지 않는다</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>홍민정</t>
+          <t>룰루 밀러</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>창비</t>
+          <t>곰출판</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>44981</v>
-      </c>
-      <c r="F37" t="inlineStr"/>
+        <v>44547</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Why Fish Don't Exist: A Story of Loss, Love, and the Hidden Order of Life</t>
+        </is>
+      </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>49,500</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>245</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>11,000원</t>
+          <t>17,000원</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>9,900</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>27300</t>
+          <t>475521</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>1-2학년 창작동화</t>
+          <t>생물학</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>11,000</t>
+          <t>17,000</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>9,900</t>
+          <t>15,300</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>550점</t>
+          <t>850점</t>
         </is>
       </c>
       <c r="P37" t="n">
-        <v>45070</v>
+        <v>260787</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>9788956608556</t>
+          <t>9788901268880</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>구의 증명</t>
+          <t>5천만 원으로 시작하는 미라클 기적의 재개발 재건축</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>최진영</t>
+          <t>장미진</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>은행나무</t>
+          <t>리더스북</t>
         </is>
       </c>
       <c r="E38" s="2" t="n">
-        <v>42093</v>
+        <v>44981</v>
       </c>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>8,000원</t>
+          <t>20,000원</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>7,200</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>156027</t>
+          <t>58143</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>한국 장편소설</t>
+          <t>부동산/경매</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>8,000</t>
+          <t>20,000</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>7,200</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>400점</t>
+          <t>1,000점</t>
         </is>
       </c>
       <c r="P38" t="n">
-        <v>88017</v>
+        <v>21180</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>9791133487523</t>
+          <t>9788988474846</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 2</t>
+          <t>SQL 자격검정 실전문제</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>이노우에 타케히코</t>
+          <t>한국데이터진흥원</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>대원</t>
+          <t>한국데이터산업진흥원</t>
         </is>
       </c>
       <c r="E39" s="2" t="n">
-        <v>43336</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版 2 </t>
-        </is>
-      </c>
+        <v>43962</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
-          <t>9.8</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>52</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>6,500원</t>
+          <t>18,000원</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>5,850</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>291171</t>
+          <t>107886</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>스포츠</t>
+          <t>SQL Server</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>6,500</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>5,850</t>
+          <t>18,000</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>320점</t>
+          <t>0점</t>
         </is>
       </c>
       <c r="P39" t="n">
-        <v>153314</v>
+        <v>59686</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>9791133487516</t>
+          <t>9791133487578</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>슬램덩크 신장재편판 1</t>
+          <t>슬램덩크 신장재편판 7</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3381,11 +3263,11 @@
         </is>
       </c>
       <c r="E40" s="2" t="n">
-        <v>43336</v>
+        <v>43361</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve">SLAM DUNK 新裝再編版  1 </t>
+          <t>SLAM DUNK 新裝再編版  7</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -3395,22 +3277,22 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>62</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>7,000원</t>
+          <t>7,500원</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>6,750</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>296085</t>
+          <t>275964</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3420,21 +3302,21 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>7,000</t>
+          <t>7,500</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>6,300</t>
+          <t>6,750</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>350점</t>
+          <t>370점</t>
         </is>
       </c>
       <c r="P40" t="n">
-        <v>156584</v>
+        <v>136280</v>
       </c>
     </row>
     <row r="41">
@@ -3488,7 +3370,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>285882</t>
+          <t>287412</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3512,7 +3394,7 @@
         </is>
       </c>
       <c r="P41" t="n">
-        <v>141019</v>
+        <v>141192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>